<commit_message>
Update discord_channel_map.xlsx with latest channel mappings
</commit_message>
<xml_diff>
--- a/discord_channel_map.xlsx
+++ b/discord_channel_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\discord_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5F14AC-64F1-4157-811F-CB5FD8EB4E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B676646-5D55-492F-BDC2-C8ABA95C561A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2545A53A-C262-40F3-B538-BEC20FAA3301}"/>
+    <workbookView xWindow="5580" yWindow="2970" windowWidth="21600" windowHeight="11295" xr2:uid="{2545A53A-C262-40F3-B538-BEC20FAA3301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>1427857797554376845</t>
   </si>
   <si>
-    <t>Medium Dog</t>
-  </si>
-  <si>
     <t>1427855363364884501</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>1427861271604367460</t>
+  </si>
+  <si>
+    <t>Mediumdog</t>
   </si>
 </sst>
 </file>
@@ -561,12 +561,12 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -732,42 +732,42 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>